<commit_message>
Agrega historia de cambios auditoria y descarga de pdf
</commit_message>
<xml_diff>
--- a/static/uploads/conexiones.xlsx
+++ b/static/uploads/conexiones.xlsx
@@ -5,23 +5,36 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carnao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Junior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7F3D29-F144-43EB-836B-E0050D86C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2EA2EC-C20B-4E14-8386-F71DAE23B619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>TULUA</t>
   </si>
@@ -233,6 +246,9 @@
     <t>Server2020@20</t>
   </si>
   <si>
+    <t>Zaq1xsw5</t>
+  </si>
+  <si>
     <t>LA VICTORIA</t>
   </si>
   <si>
@@ -293,9 +309,6 @@
     <t>15.235.36.156</t>
   </si>
   <si>
-    <t>hnss2020</t>
-  </si>
-  <si>
     <t>Server2040</t>
   </si>
   <si>
@@ -326,13 +339,10 @@
     <t>Julian$$$2023</t>
   </si>
   <si>
-    <t xml:space="preserve">1563102933	</t>
-  </si>
-  <si>
-    <t>soporte21</t>
-  </si>
-  <si>
-    <t>IPSCSR2013</t>
+    <t>hsvf2024</t>
+  </si>
+  <si>
+    <t>Servidor123</t>
   </si>
 </sst>
 </file>
@@ -762,7 +772,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,12 +784,12 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
@@ -804,7 +814,7 @@
       </c>
       <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -816,10 +826,10 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2">
-        <v>1041720654</v>
+        <v>293991913</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -830,7 +840,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -860,7 +870,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -876,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>1181438942</v>
+        <v>361662446</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>8</v>
@@ -890,7 +900,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -915,7 +925,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -930,7 +940,7 @@
         <v>743367355</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
@@ -941,7 +951,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -967,7 +977,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -978,11 +988,11 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>101</v>
+      <c r="G8" s="1">
+        <v>1563102933</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>4</v>
@@ -993,7 +1003,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1008,7 +1018,7 @@
         <v>784364917</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>4</v>
@@ -1019,7 +1029,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1027,7 +1037,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -1049,7 +1059,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1071,7 +1081,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1101,7 +1111,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1139,7 +1149,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>1477743435</v>
+        <v>539734449</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>93</v>
@@ -1153,7 +1163,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1168,7 +1178,7 @@
         <v>770371210</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>4</v>
@@ -1179,7 +1189,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1208,12 +1218,12 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1239,7 +1249,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1260,12 +1270,12 @@
         <v>4</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1289,7 +1299,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1315,7 +1325,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1326,7 +1336,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>12</v>
@@ -1345,7 +1355,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1371,7 +1381,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1379,7 +1389,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -1401,7 +1411,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1428,12 +1438,12 @@
         <v>4</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1459,12 +1469,12 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1474,7 +1484,7 @@
         <v>845975147</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>4</v>
@@ -1490,7 +1500,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1506,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1514,25 +1524,25 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="J28" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1540,7 +1550,7 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1550,7 +1560,7 @@
         <v>765138104</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1560,7 +1570,7 @@
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1580,17 +1590,17 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1631,8 +1641,8 @@
     <hyperlink ref="J18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="J26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D21" r:id="rId10" xr:uid="{14CB64C7-477B-42AC-AA60-F67CCA5AF5AC}"/>
-    <hyperlink ref="H14" r:id="rId11" xr:uid="{6B2AA7F1-D973-48D2-B160-0B955129AA70}"/>
+    <hyperlink ref="D21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>